<commit_message>
[FIX]敏捷邮件模板去掉底部的重复Copyright © The Choerodon Author. All rights reserved.
</commit_message>
<xml_diff>
--- a/src/main/resources/script/db/init-data/workflow_service/hzero_message/z_cwkf_hzero-message.xlsx
+++ b/src/main/resources/script/db/init-data/workflow_service/hzero_message/z_cwkf_hzero-message.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\hand\choerodon\workflow-service\src\main\resources\script\db\init-data\workflow_service\hzero_message\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5B41F18-9E4E-4120-9521-58BB6C5CDF59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C3DD72C-3CF3-457F-A0B3-9A1C26CF5C65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="597" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3136,232 +3136,193 @@
     <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">      
-&lt;title&gt; &lt;/title&gt;
+    <t>&lt;title&gt; &lt;/title&gt;
 &lt;!--[if !mso]&gt;&lt;!-- --&gt;
 &lt;meta http-equiv="X-UA-Compatible" content="IE=edge"&gt;
 &lt;!--&lt;![endif]--&gt;
 &lt;meta http-equiv="Content-Type" content="text/html; charset=UTF-8"&gt;
 &lt;meta name="viewport" content="width=device-width, initial-scale=1"&gt;
 &lt;style type="text/css"&gt;
-  #outlook a {
-    padding: 0;
-  }
-  .ReadMsgBody {
-    width: 100%;
-  }
-  .ExternalClass {
-    width: 100%;
-  }
-  .ExternalClass * {
-    line-height: 100%;
-  }
-  body {
-    margin: 0;
-    padding: 0;
-    -webkit-text-size-adjust: 100%;
-    -ms-text-size-adjust: 100%;
-  }
-  table,
-  td {
-    border-collapse: collapse;
-    mso-table-lspace: 0pt;
-    mso-table-rspace: 0pt;
-  }
-  img {
-    border: 0;
-    height: auto;
-    line-height: 100%;
-    outline: none;
-    text-decoration: none;
-    -ms-interpolation-mode: bicubic;
-  }
-  p {
-    display: block;
-    margin: 13px 0;
-  }
+    #outlook a {
+        padding: 0;
+    }
+    .ReadMsgBody {
+        width: 100%;
+    }
+    .ExternalClass {
+        width: 100%;
+    }
+    .ExternalClass * {
+        line-height: 100%;
+    }
+    body {
+        margin: 0;
+        padding: 0;
+        -webkit-text-size-adjust: 100%;
+        -ms-text-size-adjust: 100%;
+    }
+    table,
+    td {
+        border-collapse: collapse;
+        mso-table-lspace: 0pt;
+        mso-table-rspace: 0pt;
+    }
+    img {
+        border: 0;
+        height: auto;
+        line-height: 100%;
+        outline: none;
+        text-decoration: none;
+        -ms-interpolation-mode: bicubic;
+    }
+    p {
+        display: block;
+        margin: 13px 0;
+    }
 &lt;/style&gt;
 &lt;!--[if !mso]&gt;&lt;!--&gt;
 &lt;style type="text/css"&gt;
-  @media only screen and (max-width:480px) {
-    @-ms-viewport {
-      width: 320px;
+    @media only screen and (max-width:480px) {
+        @-ms-viewport {
+            width: 320px;
+        }
+        @viewport {
+            width: 320px;
+        }
     }
-    @viewport {
-      width: 320px;
-    }
-  }
 &lt;/style&gt;
 &lt;!--&lt;![endif]--&gt;
 &lt;!--[if mso]&gt;
 &lt;xml&gt;
-  &lt;o:OfficeDocumentSettings&gt;
-    &lt;o:AllowPNG/&gt;
-    &lt;o:PixelsPerInch&gt;96&lt;/o:PixelsPerInch&gt;
-  &lt;/o:OfficeDocumentSettings&gt;
+    &lt;o:OfficeDocumentSettings&gt;
+        &lt;o:AllowPNG/&gt;
+        &lt;o:PixelsPerInch&gt;96&lt;/o:PixelsPerInch&gt;
+    &lt;/o:OfficeDocumentSettings&gt;
 &lt;/xml&gt;
 &lt;![endif]--&gt;
 &lt;!--[if lte mso 11]&gt;
 &lt;style type="text/css"&gt;
-  .outlook-group-fix { width:100% !important; }
+    .outlook-group-fix { width:100% !important; }
 &lt;/style&gt;
 &lt;![endif]--&gt;
 &lt;!--[if !mso]&gt;&lt;!--&gt;
 &lt;link href="https://fonts.googleapis.com/css?family=Ubuntu:300,400,500,700" rel="stylesheet" type="text/css"&gt;
 &lt;style type="text/css"&gt;
-  @import url(https://fonts.googleapis.com/css?family=Ubuntu:300,400,500,700);
+    @import url(https://fonts.googleapis.com/css?family=Ubuntu:300,400,500,700);
 &lt;/style&gt;
 &lt;!--&lt;![endif]--&gt;
 &lt;style type="text/css"&gt;
-  @media only screen and (min-width:480px) {
-    .mj-column-per-100 {
-      width: 100% !important;
-      max-width: 100%;
+    @media only screen and (min-width:480px) {
+        .mj-column-per-100 {
+            width: 100% !important;
+            max-width: 100%;
+        }
     }
-  }
 &lt;/style&gt;
 &lt;style type="text/css"&gt;
 &lt;/style&gt;
-&lt;/head&gt;&lt;body&gt;&lt;div style=""&gt;
-&lt;!--[if mso | IE]&gt;
-&lt;table
-        align="center" border="0" cellpadding="0" cellspacing="0" class="" style="width:782px;" width="782"
-&gt;
-  &lt;tr&gt;
-    &lt;td style="line-height:0px;font-size:0px;mso-line-height-rule:exactly;"&gt;
-&lt;![endif]--&gt;
-&lt;div style="Margin:0px auto;max-width:782px;"&gt;
-  &lt;table align="center" border="0" cellpadding="0" cellspacing="0" role="presentation" style="width:100%;"&gt;
-    &lt;tbody&gt;
-    &lt;tr&gt;
-      &lt;td style="direction:ltr;font-size:0px;padding:20px 0;text-align:center;vertical-align:top;"&gt;
+&lt;/head&gt;
+&lt;body&gt;
+    &lt;div style=""&gt;
         &lt;!--[if mso | IE]&gt;
-        &lt;table role="presentation" border="0" cellpadding="0" cellspacing="0"&gt;
-          &lt;tr&gt;
-            &lt;td
-                    class="" style="vertical-align:top;width:782px;"
-            &gt;
-        &lt;![endif]--&gt;
-        &lt;div class="mj-column-per-100 outlook-group-fix" style="font-size:13px;text-align:left;direction:ltr;display:inline-block;vertical-align:top;width:100%;"&gt;
-          &lt;table border="0" cellpadding="0" cellspacing="0" role="presentation" style="vertical-align:top;" width="100%"&gt;
-            &lt;tbody&gt;&lt;tr&gt;
-              &lt;td align="left" style="padding: 10px 25px; word-break: break-word;"&gt;
-                &lt;div style="line-height: 1; text-align: left;"&gt;
-                  &lt;div style="width: 782px; background: rgb(255, 255, 255); margin: 0px auto;"&gt;
-                    &lt;div style="margin-top: 60px;color: rgb(0, 0, 0);font-family: Ubuntu, Helvetica, Arial, sans-serif;font-size: 13px;height: 55px;background-color: rgb(255, 255, 255);"&gt;
-                      &lt;table style="width: 100%;"&gt;
-                        &lt;tbody&gt;&lt;tr&gt;
-                          &lt;td style="padding-bottom: 10px;vertical-align: bottom;"&gt;
-                            &lt;table style="width: 100%;"&gt;
-                              &lt;tbody&gt;&lt;tr&gt;
-                                &lt;td style="width:238px;"&gt; &lt;img height="auto" src="https://file.choerodon.com.cn/static/zknow-logo.jpg" style="border:0;display:block;outline:none;text-decoration:none;height:auto;width:100%;" width="190"&gt; &lt;/td&gt;
-                              &lt;td style="text-align: right;vertical-align: middle;font-family: PingFangSC-Regular;padding-right: 0px;font-size: 14px;color: rgba(15,19,88,0.65);"&gt; 猪齿鱼 数智化开发管理平台&lt;/td&gt;&lt;/tr&gt;
-                            &lt;/tbody&gt;&lt;/table&gt;
-                          &lt;/td&gt;&lt;td&gt;
-                          &lt;/td&gt;
-                        &lt;/tr&gt;
-                      &lt;/tbody&gt;&lt;/table&gt;
-                    &lt;/div&gt;
-                    &lt;div style="border-width: 1px 0px;border-bottom-style: solid;border-bottom-color: #D9E6F2;border-top-style: solid;border-top-color: #D9E6F2;border-radius: 2px;background: rgb(255, 255, 255);"&gt;
-                      &lt;div style="margin: 0px 10px"&gt;
-                       &lt;p style="color: #0F1358;font-family: PingFangSC-Regular;font-size: 16px;margin-top: 0px;padding-top: 20px;padding-bottom: 14px;margin-bottom: 0px;"&gt;猪齿鱼通知-工作流待办事项&lt;/p&gt;
-                        &lt;p style="color: #0F1358;font-family: PingFangSC-Regular;font-size: 14px;text-align: justify;margin-bottom: 0px;margin-top: 0px; line-height: 24px;"&gt;您好，您有一个新的待办事项需要&lt;a href="${domainName}/#/workbench?id=${tenantId}&amp;amp;type=organization" style="text-decoration:none;color: #5365EA" target="_blank"&gt;处理&lt;/a&gt;。&lt;/p&gt;
-                        &lt;p style="color: #0F1358;font-family: PingFangSC-Regular;font-size: 14px;text-align: justify;margin-bottom: 0px;margin-top: 0px; line-height: 24px;"&gt;待办名称：【${backlog_num}】${summary}&lt;/p&gt;
-                      &lt;/div&gt;
-                      &lt;br&gt;
-                    &lt;/div&gt;
-                    &lt;div style="color: rgb(0, 0, 0);font-family: PingFangSC-Regular;font-size: 13px;border-bottom-style: solid;border-bottom-color: #D9E6F2;border-width: 1px;"&gt;
-                      &lt;div style="text-align: justify;"&gt;
-                        &lt;table style="height: 148px;width: 100%;"&gt;
-                          &lt;tbody&gt;&lt;tr&gt;
-                            &lt;td&gt;
-                              &lt;div style="/* padding-top: 1px; */margin-left: 10px;/* height: 90px; *//* margin-top: 28px; */vertical-align: top;"&gt;
-                                &lt;p style="
-    font-size: 13px;
-    color: rgba(15,19,88,0.80);
-    letter-spacing: 0;
-    text-align: left;
-    margin-bottom: 6px;
-    margin-top: 0;
-    border-width: 1px;
-    "&gt; 此邮件为系统邮件，请勿回复。 &lt;/p&gt;
-                                &lt;p style="
-    font-size: 13px;
-    color: rgba(15,19,88,0.80);
-    letter-spacing: 0;
-    text-align: left;
-    margin-bottom: 6px;
-    margin-top: 0;
-    "&gt; 如果您还尚未掌握Choerodon猪齿鱼的功能和操作，可以访问 &lt;a style="text-decoration:none;font-size: 12px;color: #5365EA;" href="https://zhuchiyu.zknow.com/" target="_blank"&gt;Choerodon官网&lt;/a&gt; 或 &lt;a style="text-decoration:none;font-size: 12px;color: #5365EA;" href="https://www.zknow.com/choerodonDoc/%E4%BB%8B%E7%BB%8D/" target="_blank"&gt;帮助文档&lt;/a&gt;。 &lt;/p&gt;
-                                &lt;p style="font-size: 13px;
-    color: rgba(15,19,88,0.80);
-    letter-spacing: 0;
-    text-align: left;
-    margin-bottom: 6px;
-    margin-top: 0;"&gt; 如果您需要任何帮助或者提供反馈, 请访问 &lt;a style="text-decoration:none;font-size: 12px;color: #5365EA;" href="https://openforum.hand-china.com/" target="_blank"&gt;Choerodon论坛&lt;/a&gt;。 &lt;/p&gt;
-                                &lt;p style="font-size: 13px;
-    color: rgba(15,19,88,0.80);
-    letter-spacing: 0;
-    text-align: left;
-    margin-bottom: 6px;
-        margin-top: 0;"&gt;您也可以通过以下方式与我们联系：官方邮箱&lt;a href="mailto:marketing@zknow.com" style="text-decoration:none;font-size: 12px;color: #5365EA;"  target="_blank" rel="noopener  norefferrer"&gt;marketing@zknow.com&lt;/a&gt;，咨询热线 400 800 2077&lt;/p&gt;
-                              &lt;/div&gt;
-                            &lt;/td&gt;
-                          &lt;td style="padding-left: 19px;"&gt;
-                              &lt;table&gt;
-                                &lt;tbody&gt;&lt;tr&gt;
-                                  &lt;td&gt; &lt;img height="auto" style="border: 1px solid #D9E6F2;display:block;outline:none;text-decoration:none;height:80px;width:80px;" src="https://file.choerodon.com.cn/static/xiaozhushou.png"&gt; &lt;/td&gt;&lt;/tr&gt;
-                                &lt;tr&gt;
-                                  &lt;td style="text-align: center;font-family: PingFangSC-Regular;font-size: 13px;color: rgba(15,19,88,0.65);"&gt;官方小助手&lt;/td&gt;
-                                &lt;/tr&gt;
-                              &lt;/tbody&gt;&lt;/table&gt;
-                            &lt;/td&gt;&lt;td style="padding-left: 19px;"&gt;
-                              &lt;table&gt;
-                                &lt;tbody&gt;&lt;tr&gt;
-                                  &lt;td&gt; &lt;img height="auto" style="border: 1px solid #D9E6F2;display:block;outline:none;text-decoration:none;height:80px;width:80px;" src="https://file.choerodon.com.cn/static/gongzhonghao.png"&gt; &lt;/td&gt;&lt;/tr&gt;
-                                &lt;tr&gt;
-                                  &lt;td style="text-align: center;font-family: PingFangSC-Regular;font-size: 13px;color: rgba(15,19,88,0.65);"&gt;微信公众号&lt;/td&gt;
-                                &lt;/tr&gt;
-                              &lt;/tbody&gt;&lt;/table&gt;
-                            &lt;/td&gt;&lt;/tr&gt;
-                        &lt;/tbody&gt;&lt;/table&gt;
-                      &lt;/div&gt;
-                    &lt;/div&gt;
-                    &lt;div style="color: rgb(0, 0, 0);font-family: PingFangSC-Regular;font-size: 13px;width: 782px;height: 34px;"&gt;
-                      &lt;p style="
-    opacity: 0.8;
-    font-size: 10px;
-    color: rgba(15,19,88,0.65);
-    text-align: center;
-    display: inline-block;
-    line-height: 34px;
-    width: 100%;
-    margin: 0 auto;
-    "&gt;Copyright © The Choerodon Author. All rights reserved.&lt;/p&gt;
-                    &lt;/div&gt;
-                  &lt;/div&gt;
-                &lt;/div&gt;
-              &lt;/td&gt;
-            &lt;/tr&gt;
-          &lt;/tbody&gt;&lt;/table&gt;
-        &lt;/div&gt;
-        &lt;!--[if mso | IE]&gt;
+    &lt;table
+            align="center" border="0" cellpadding="0" cellspacing="0" class="" style="width:782px;" width="782"
+    &gt;
+        &lt;tr&gt;
+            &lt;td style="line-height:0px;font-size:0px;mso-line-height-rule:exactly;"&gt;
+    &lt;![endif]--&gt;
+        &lt;div style="Margin:0px auto;max-width:782px;"&gt;
+            &lt;table align="center" border="0" cellpadding="0" cellspacing="0" role="presentation" style="width:100%;"&gt;
+                &lt;tbody&gt;
+                    &lt;tr&gt;
+                        &lt;td style="direction:ltr;font-size:0px;padding:20px 0;text-align:center;vertical-align:top;"&gt;
+                            &lt;!--[if mso | IE]&gt;
+                    &lt;table role="presentation" border="0" cellpadding="0" cellspacing="0"&gt;
+                        &lt;tr&gt;
+                            &lt;td
+                                    class="" style="vertical-align:top;width:782px;"
+                            &gt;
+                    &lt;![endif]--&gt;
+                            &lt;div class="mj-column-per-100 outlook-group-fix"
+                                style="font-size:13px;text-align:left;direction:ltr;display:inline-block;vertical-align:top;width:100%;"&gt;
+                                &lt;table border="0" cellpadding="0" cellspacing="0" role="presentation"
+                                    style="vertical-align:top;" width="100%"&gt;
+                                    &lt;tbody&gt;
+                                        &lt;tr&gt;
+                                            &lt;td align="left" style="padding: 10px 25px; word-break: break-word;"&gt;
+                                                &lt;div style="line-height: 1; text-align: left;"&gt;
+                                                    &lt;div
+                                                        style="width: 782px; background: rgb(255, 255, 255); margin: 0px auto;"&gt;
+                                                        &lt;div
+                                                            style="margin-top: 60px;color: rgb(0, 0, 0);font-family: Ubuntu, Helvetica, Arial, sans-serif;font-size: 13px;height: 55px;background-color: rgb(255, 255, 255);"&gt;
+                                                            &lt;table style="width: 100%;"&gt;
+                                                                &lt;tbody&gt;
+                                                                    &lt;tr&gt;
+                                                                        &lt;td
+                                                                            style="padding-bottom: 20px;vertical-align: bottom;"&gt;
+                                                                            &lt;table style="width: 100%;"&gt;
+                                                                                &lt;tbody&gt;
+                                                                                    &lt;tr&gt;
+                                                                                        &lt;td&gt; &lt;img src="${choerodonLogo}"
+                                                                                                style="border:0;display:block;outline:none;text-decoration:none;height: 36px ; width: auto"&gt;
+                                                                                        &lt;/td&gt;
+                                                                                        &lt;td
+                                                                                            style="text-align: right;vertical-align: middle;font-family: PingFangSC-Regular;padding-right: 0px;font-size: 14px;color: rgba(15,19,88,0.65);"&gt;
+                                                                                            ${choerodonSlogan}&lt;/td&gt;
+                                                                                    &lt;/tr&gt;
+                                                                                &lt;/tbody&gt;
+                                                                            &lt;/table&gt;
+                                                                        &lt;/td&gt;
+                                                                        &lt;td&gt;
+                                                                        &lt;/td&gt;
+                                                                    &lt;/tr&gt;
+                                                                &lt;/tbody&gt;
+                                                            &lt;/table&gt;
+                                                        &lt;/div&gt;
+                                                        &lt;div
+                                                            style="border-width: 1px 0px;border-bottom-style: solid;border-bottom-color: #D9E6F2;border-top-style: solid;border-top-color: #D9E6F2;border-radius: 2px;background: rgb(255, 255, 255);"&gt;
+                                                            &lt;div style="margin: 0px 10px"&gt;
+                                                                &lt;p
+                                                                    style="color: #0F1358;font-family: PingFangSC-Regular;font-size: 16px;margin-top: 0px;padding-top: 20px;padding-bottom: 14px;margin-bottom: 0px;"&gt;
+                                                                    猪齿鱼通知-工作流待办事项&lt;/p&gt;
+                                                                &lt;p
+                                                                    style="color: #0F1358;font-family: PingFangSC-Regular;font-size: 14px;text-align: justify;margin-bottom: 0px;margin-top: 0px; line-height: 24px;"&gt;
+                                                                    您好，您有一个新的待办事项需要&lt;a
+                                                                        href="${domainName}/#/workbench?id=${tenantId}&amp;amp;type=organization"
+                                                                        style="text-decoration:none;color: #5365EA"
+                                                                        target="_blank"&gt;处理&lt;/a&gt;。&lt;/p&gt;
+                                                                &lt;p
+                                                                    style="color: #0F1358;font-family: PingFangSC-Regular;font-size: 14px;text-align: justify;margin-bottom: 0px;margin-top: 0px; line-height: 24px;"&gt;
+                                                                    待办名称：【${backlog_num}】${summary}&lt;/p&gt;
+                                                            &lt;/div&gt;
+                                                            &lt;br&gt;
+                                                        &lt;/div&gt;
+                                                        ${choerodonFooter}
+                                                    &lt;/div&gt;
+                                                &lt;/div&gt;
+                                            &lt;/td&gt;
+                                        &lt;/tr&gt;
+                                    &lt;/tbody&gt;
+                                &lt;/table&gt;
+                            &lt;/div&gt;
+                            &lt;!--[if mso | IE]&gt;
         &lt;/td&gt;
         &lt;/tr&gt;
         &lt;/table&gt;
         &lt;![endif]--&gt;
-      &lt;/td&gt;
-    &lt;/tr&gt;
-    &lt;/tbody&gt;
-  &lt;/table&gt;&lt;br&gt;
-&lt;/div&gt;
-&lt;!--[if mso | IE]&gt;
+                        &lt;/td&gt;
+                    &lt;/tr&gt;
+                &lt;/tbody&gt;
+            &lt;/table&gt;
+            &lt;br /&gt;
+        &lt;/div&gt;
+        &lt;!--[if mso | IE]&gt;
 &lt;/td&gt;
 &lt;/tr&gt;
 &lt;/table&gt;
 &lt;![endif]--&gt;
-&lt;/div&gt;
-  </t>
+    &lt;/div&gt;
+&lt;/body&gt;</t>
     <phoneticPr fontId="15" type="noConversion"/>
   </si>
 </sst>
@@ -3865,7 +3826,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3873,9 +3834,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3890,31 +3850,30 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3959,25 +3918,20 @@
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -4333,7 +4287,7 @@
     <col min="1" max="1" width="15.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.35546875" style="2" customWidth="1"/>
     <col min="3" max="3" width="28.140625" customWidth="1"/>
-    <col min="4" max="4" width="35.35546875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="35.35546875" customWidth="1"/>
     <col min="5" max="5" width="38.5703125" customWidth="1"/>
     <col min="6" max="6" width="23.42578125" customWidth="1"/>
     <col min="7" max="7" width="21.5703125" customWidth="1"/>
@@ -4347,79 +4301,79 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="64.5" customHeight="1">
-      <c r="A1" s="4"/>
-      <c r="C1" s="76" t="s">
+      <c r="A1" s="3"/>
+      <c r="C1" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="E2" s="6"/>
+      <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:8" ht="49.5" customHeight="1">
-      <c r="C3" s="75" t="s">
+      <c r="C3" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="75"/>
-      <c r="E3" s="77" t="s">
+      <c r="D3" s="68"/>
+      <c r="E3" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="77"/>
-      <c r="G3" s="77"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="C4" s="78" t="s">
+      <c r="C4" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="78"/>
-      <c r="E4" s="7" t="s">
+      <c r="D4" s="71"/>
+      <c r="E4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="8" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="4"/>
+      <c r="A5" s="3"/>
       <c r="C5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="15"/>
+      <c r="E8" s="13"/>
     </row>
     <row r="9" spans="1:8" ht="49.5">
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="16" t="s">
         <v>15</v>
       </c>
       <c r="F9" t="s">
@@ -4427,56 +4381,54 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="49.5">
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="E10" s="16" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="66">
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="18" t="s">
+      <c r="E11" s="16" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="20" t="s">
+      <c r="E12" s="18" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="C13" s="13"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="15"/>
+      <c r="C13" s="12"/>
+      <c r="E13" s="13"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="C14" s="13"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="15"/>
+      <c r="C14" s="12"/>
+      <c r="E14" s="13"/>
     </row>
     <row r="15" spans="1:8" ht="33">
-      <c r="C15" s="21" t="s">
+      <c r="C15" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="22" t="s">
+      <c r="D15" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="23" t="s">
+      <c r="E15" s="21" t="s">
         <v>28</v>
       </c>
     </row>
@@ -4486,64 +4438,64 @@
       </c>
     </row>
     <row r="19" spans="3:5">
-      <c r="C19" s="79" t="s">
+      <c r="C19" s="72" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="79"/>
-      <c r="E19" s="79"/>
+      <c r="D19" s="72"/>
+      <c r="E19" s="72"/>
     </row>
     <row r="20" spans="3:5">
-      <c r="C20" s="24" t="s">
+      <c r="C20" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="5" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="21" spans="3:5">
-      <c r="C21" s="24" t="s">
+      <c r="C21" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="22" spans="3:5">
-      <c r="C22" s="24" t="s">
+      <c r="C22" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="23" spans="3:5">
-      <c r="C23" s="24" t="s">
+      <c r="C23" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="25" spans="3:5" ht="69" customHeight="1">
-      <c r="C25" s="25" t="s">
+      <c r="C25" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="D25" s="75" t="s">
+      <c r="D25" s="68" t="s">
         <v>40</v>
       </c>
-      <c r="E25" s="75"/>
+      <c r="E25" s="68"/>
     </row>
     <row r="26" spans="3:5" ht="14.25" customHeight="1">
-      <c r="C26" s="14" t="s">
+      <c r="C26" t="s">
         <v>41</v>
       </c>
-      <c r="D26" s="75" t="s">
+      <c r="D26" s="68" t="s">
         <v>42</v>
       </c>
-      <c r="E26" s="75"/>
+      <c r="E26" s="68"/>
     </row>
     <row r="27" spans="3:5" ht="49.5">
-      <c r="C27" s="26" t="s">
+      <c r="C27" s="24" t="s">
         <v>43</v>
       </c>
     </row>
@@ -4568,38 +4520,37 @@
   <dimension ref="A1:Q165"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="6" max="6" width="39.42578125" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="69"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="28" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:17">
-      <c r="E4" s="31" t="s">
+      <c r="E4" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="F4" s="32" t="s">
+      <c r="F4" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="G4" s="33" t="s">
+      <c r="G4" s="31" t="s">
         <v>49</v>
       </c>
     </row>
@@ -4613,13 +4564,13 @@
       <c r="C7" t="s">
         <v>52</v>
       </c>
-      <c r="D7" s="41" t="s">
+      <c r="D7" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="E7" s="42" t="s">
+      <c r="E7" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="F7" s="43" t="s">
+      <c r="F7" s="41" t="s">
         <v>55</v>
       </c>
       <c r="G7" t="s">
@@ -4628,7 +4579,7 @@
       <c r="H7" t="s">
         <v>57</v>
       </c>
-      <c r="I7" s="69" t="s">
+      <c r="I7" t="s">
         <v>58</v>
       </c>
       <c r="J7" t="s">
@@ -4643,13 +4594,13 @@
       <c r="M7" t="s">
         <v>62</v>
       </c>
-      <c r="N7" s="44" t="s">
+      <c r="N7" s="42" t="s">
         <v>63</v>
       </c>
       <c r="O7" t="s">
         <v>64</v>
       </c>
-      <c r="P7" s="45" t="s">
+      <c r="P7" s="43" t="s">
         <v>65</v>
       </c>
       <c r="Q7" t="s">
@@ -4660,16 +4611,16 @@
       <c r="E8" t="s">
         <v>67</v>
       </c>
-      <c r="F8" s="71" t="s">
+      <c r="F8" s="67" t="s">
         <v>233</v>
       </c>
-      <c r="G8" s="72" t="s">
+      <c r="G8" t="s">
         <v>86</v>
       </c>
-      <c r="H8" s="72" t="s">
+      <c r="H8" t="s">
         <v>87</v>
       </c>
-      <c r="I8" s="73" t="s">
+      <c r="I8" s="67" t="s">
         <v>234</v>
       </c>
       <c r="J8" t="s">
@@ -4695,16 +4646,16 @@
       <c r="E9" t="s">
         <v>76</v>
       </c>
-      <c r="F9" s="71" t="s">
+      <c r="F9" s="67" t="s">
         <v>235</v>
       </c>
-      <c r="G9" s="72" t="s">
+      <c r="G9" t="s">
         <v>90</v>
       </c>
-      <c r="H9" s="72" t="s">
+      <c r="H9" t="s">
         <v>91</v>
       </c>
-      <c r="I9" s="73" t="s">
+      <c r="I9" s="67" t="s">
         <v>211</v>
       </c>
       <c r="J9" t="s">
@@ -4730,16 +4681,16 @@
       <c r="E10" t="s">
         <v>80</v>
       </c>
-      <c r="F10" s="71" t="s">
+      <c r="F10" s="67" t="s">
         <v>236</v>
       </c>
-      <c r="G10" s="72" t="s">
+      <c r="G10" t="s">
         <v>94</v>
       </c>
-      <c r="H10" s="72" t="s">
+      <c r="H10" t="s">
         <v>95</v>
       </c>
-      <c r="I10" s="73" t="s">
+      <c r="I10" s="67" t="s">
         <v>212</v>
       </c>
       <c r="J10" t="s">
@@ -4765,16 +4716,16 @@
       <c r="E11" t="s">
         <v>84</v>
       </c>
-      <c r="F11" s="71" t="s">
+      <c r="F11" s="67" t="s">
         <v>237</v>
       </c>
-      <c r="G11" s="72" t="s">
+      <c r="G11" t="s">
         <v>98</v>
       </c>
-      <c r="H11" s="72" t="s">
+      <c r="H11" t="s">
         <v>99</v>
       </c>
-      <c r="I11" s="73" t="s">
+      <c r="I11" s="67" t="s">
         <v>213</v>
       </c>
       <c r="J11" t="s">
@@ -4800,16 +4751,16 @@
       <c r="E12" t="s">
         <v>88</v>
       </c>
-      <c r="F12" s="73" t="s">
+      <c r="F12" s="67" t="s">
         <v>219</v>
       </c>
-      <c r="G12" s="74" t="s">
+      <c r="G12" t="s">
         <v>110</v>
       </c>
-      <c r="H12" s="74" t="s">
+      <c r="H12" t="s">
         <v>111</v>
       </c>
-      <c r="I12" s="73" t="s">
+      <c r="I12" s="67" t="s">
         <v>238</v>
       </c>
       <c r="K12" t="s">
@@ -4832,16 +4783,16 @@
       <c r="E13" t="s">
         <v>92</v>
       </c>
-      <c r="F13" s="73" t="s">
+      <c r="F13" s="67" t="s">
         <v>239</v>
       </c>
-      <c r="G13" s="74" t="s">
+      <c r="G13" t="s">
         <v>199</v>
       </c>
-      <c r="H13" s="74" t="s">
+      <c r="H13" t="s">
         <v>209</v>
       </c>
-      <c r="I13" s="73" t="s">
+      <c r="I13" s="67" t="s">
         <v>265</v>
       </c>
       <c r="K13" t="s">
@@ -4864,16 +4815,16 @@
       <c r="E14" t="s">
         <v>96</v>
       </c>
-      <c r="F14" s="71" t="s">
+      <c r="F14" s="67" t="s">
         <v>240</v>
       </c>
-      <c r="G14" s="72" t="s">
+      <c r="G14" t="s">
         <v>69</v>
       </c>
-      <c r="H14" s="72" t="s">
+      <c r="H14" t="s">
         <v>69</v>
       </c>
-      <c r="I14" s="73" t="s">
+      <c r="I14" s="67" t="s">
         <v>214</v>
       </c>
       <c r="J14" t="s">
@@ -4899,16 +4850,16 @@
       <c r="E15" t="s">
         <v>100</v>
       </c>
-      <c r="F15" s="71" t="s">
+      <c r="F15" s="67" t="s">
         <v>241</v>
       </c>
-      <c r="G15" s="72" t="s">
+      <c r="G15" t="s">
         <v>78</v>
       </c>
-      <c r="H15" s="72" t="s">
+      <c r="H15" t="s">
         <v>79</v>
       </c>
-      <c r="I15" s="73" t="s">
+      <c r="I15" s="67" t="s">
         <v>215</v>
       </c>
       <c r="J15" t="s">
@@ -4934,16 +4885,16 @@
       <c r="E16" t="s">
         <v>104</v>
       </c>
-      <c r="F16" s="71" t="s">
+      <c r="F16" s="67" t="s">
         <v>242</v>
       </c>
-      <c r="G16" s="72" t="s">
+      <c r="G16" t="s">
         <v>82</v>
       </c>
-      <c r="H16" s="72" t="s">
+      <c r="H16" t="s">
         <v>83</v>
       </c>
-      <c r="I16" s="73" t="s">
+      <c r="I16" s="67" t="s">
         <v>243</v>
       </c>
       <c r="J16" t="s">
@@ -4969,16 +4920,16 @@
       <c r="E17" t="s">
         <v>108</v>
       </c>
-      <c r="F17" s="71" t="s">
+      <c r="F17" s="67" t="s">
         <v>244</v>
       </c>
-      <c r="G17" s="72" t="s">
+      <c r="G17" t="s">
         <v>102</v>
       </c>
-      <c r="H17" s="72" t="s">
+      <c r="H17" t="s">
         <v>103</v>
       </c>
-      <c r="I17" s="73" t="s">
+      <c r="I17" s="67" t="s">
         <v>216</v>
       </c>
       <c r="J17" t="s">
@@ -5004,16 +4955,16 @@
       <c r="E18" t="s">
         <v>112</v>
       </c>
-      <c r="F18" s="71" t="s">
+      <c r="F18" s="67" t="s">
         <v>245</v>
       </c>
-      <c r="G18" s="72" t="s">
+      <c r="G18" t="s">
         <v>106</v>
       </c>
-      <c r="H18" s="72" t="s">
+      <c r="H18" t="s">
         <v>107</v>
       </c>
-      <c r="I18" s="73" t="s">
+      <c r="I18" s="67" t="s">
         <v>210</v>
       </c>
       <c r="J18" t="s">
@@ -5039,16 +4990,16 @@
       <c r="E19" t="s">
         <v>117</v>
       </c>
-      <c r="F19" s="71" t="s">
+      <c r="F19" s="67" t="s">
         <v>246</v>
       </c>
-      <c r="G19" s="72" t="s">
+      <c r="G19" t="s">
         <v>113</v>
       </c>
-      <c r="H19" s="72" t="s">
+      <c r="H19" t="s">
         <v>114</v>
       </c>
-      <c r="I19" s="73" t="s">
+      <c r="I19" s="67" t="s">
         <v>217</v>
       </c>
       <c r="J19" t="s">
@@ -5074,16 +5025,16 @@
       <c r="E20" t="s">
         <v>189</v>
       </c>
-      <c r="F20" s="71" t="s">
+      <c r="F20" s="67" t="s">
         <v>246</v>
       </c>
-      <c r="G20" s="72" t="s">
+      <c r="G20" t="s">
         <v>118</v>
       </c>
-      <c r="H20" s="72" t="s">
+      <c r="H20" t="s">
         <v>118</v>
       </c>
-      <c r="I20" s="73" t="s">
+      <c r="I20" s="67" t="s">
         <v>218</v>
       </c>
       <c r="J20" t="s">
@@ -5109,16 +5060,16 @@
       <c r="E21" t="s">
         <v>190</v>
       </c>
-      <c r="F21" s="71" t="s">
+      <c r="F21" s="67" t="s">
         <v>247</v>
       </c>
-      <c r="G21" s="72" t="s">
+      <c r="G21" t="s">
         <v>200</v>
       </c>
-      <c r="H21" s="72" t="s">
+      <c r="H21" t="s">
         <v>111</v>
       </c>
-      <c r="I21" s="73" t="s">
+      <c r="I21" s="67" t="s">
         <v>248</v>
       </c>
       <c r="J21" t="s">
@@ -5144,16 +5095,16 @@
       <c r="E22" t="s">
         <v>191</v>
       </c>
-      <c r="F22" s="71" t="s">
+      <c r="F22" s="67" t="s">
         <v>249</v>
       </c>
-      <c r="G22" s="72" t="s">
+      <c r="G22" t="s">
         <v>201</v>
       </c>
-      <c r="H22" s="72" t="s">
+      <c r="H22" t="s">
         <v>83</v>
       </c>
-      <c r="I22" s="73" t="s">
+      <c r="I22" s="67" t="s">
         <v>250</v>
       </c>
       <c r="J22" t="s">
@@ -5179,16 +5130,16 @@
       <c r="E23" t="s">
         <v>192</v>
       </c>
-      <c r="F23" s="71" t="s">
+      <c r="F23" s="67" t="s">
         <v>251</v>
       </c>
-      <c r="G23" s="72" t="s">
+      <c r="G23" t="s">
         <v>202</v>
       </c>
-      <c r="H23" s="72" t="s">
+      <c r="H23" t="s">
         <v>87</v>
       </c>
-      <c r="I23" s="73" t="s">
+      <c r="I23" s="67" t="s">
         <v>252</v>
       </c>
       <c r="J23" t="s">
@@ -5214,16 +5165,16 @@
       <c r="E24" t="s">
         <v>193</v>
       </c>
-      <c r="F24" s="71" t="s">
+      <c r="F24" s="67" t="s">
         <v>253</v>
       </c>
-      <c r="G24" s="72" t="s">
+      <c r="G24" t="s">
         <v>203</v>
       </c>
-      <c r="H24" s="72" t="s">
+      <c r="H24" t="s">
         <v>91</v>
       </c>
-      <c r="I24" s="73" t="s">
+      <c r="I24" s="67" t="s">
         <v>254</v>
       </c>
       <c r="J24" t="s">
@@ -5249,16 +5200,16 @@
       <c r="E25" t="s">
         <v>194</v>
       </c>
-      <c r="F25" s="71" t="s">
+      <c r="F25" s="67" t="s">
         <v>255</v>
       </c>
-      <c r="G25" s="72" t="s">
+      <c r="G25" t="s">
         <v>204</v>
       </c>
-      <c r="H25" s="72" t="s">
+      <c r="H25" t="s">
         <v>95</v>
       </c>
-      <c r="I25" s="73" t="s">
+      <c r="I25" s="67" t="s">
         <v>256</v>
       </c>
       <c r="J25" t="s">
@@ -5284,16 +5235,16 @@
       <c r="E26" t="s">
         <v>195</v>
       </c>
-      <c r="F26" s="71" t="s">
+      <c r="F26" s="67" t="s">
         <v>257</v>
       </c>
-      <c r="G26" s="72" t="s">
+      <c r="G26" t="s">
         <v>205</v>
       </c>
-      <c r="H26" s="72" t="s">
+      <c r="H26" t="s">
         <v>99</v>
       </c>
-      <c r="I26" s="73" t="s">
+      <c r="I26" s="67" t="s">
         <v>258</v>
       </c>
       <c r="J26" t="s">
@@ -5319,16 +5270,16 @@
       <c r="E27" t="s">
         <v>196</v>
       </c>
-      <c r="F27" s="71" t="s">
+      <c r="F27" s="67" t="s">
         <v>259</v>
       </c>
-      <c r="G27" s="72" t="s">
+      <c r="G27" t="s">
         <v>206</v>
       </c>
-      <c r="H27" s="72" t="s">
+      <c r="H27" t="s">
         <v>79</v>
       </c>
-      <c r="I27" s="73" t="s">
+      <c r="I27" s="67" t="s">
         <v>260</v>
       </c>
       <c r="J27" t="s">
@@ -5354,16 +5305,16 @@
       <c r="E28" t="s">
         <v>197</v>
       </c>
-      <c r="F28" s="71" t="s">
+      <c r="F28" s="67" t="s">
         <v>261</v>
       </c>
-      <c r="G28" s="72" t="s">
+      <c r="G28" t="s">
         <v>207</v>
       </c>
-      <c r="H28" s="72" t="s">
+      <c r="H28" t="s">
         <v>103</v>
       </c>
-      <c r="I28" s="73" t="s">
+      <c r="I28" s="67" t="s">
         <v>262</v>
       </c>
       <c r="J28" t="s">
@@ -5389,16 +5340,16 @@
       <c r="E29" t="s">
         <v>198</v>
       </c>
-      <c r="F29" s="71" t="s">
+      <c r="F29" s="67" t="s">
         <v>263</v>
       </c>
-      <c r="G29" s="72" t="s">
+      <c r="G29" t="s">
         <v>208</v>
       </c>
-      <c r="H29" s="72" t="s">
+      <c r="H29" t="s">
         <v>107</v>
       </c>
-      <c r="I29" s="73" t="s">
+      <c r="I29" s="67" t="s">
         <v>264</v>
       </c>
       <c r="J29" t="s">
@@ -5430,22 +5381,22 @@
       <c r="C31" t="s">
         <v>119</v>
       </c>
-      <c r="D31" s="46" t="s">
+      <c r="D31" s="44" t="s">
         <v>120</v>
       </c>
-      <c r="E31" s="47" t="s">
+      <c r="E31" s="45" t="s">
         <v>121</v>
       </c>
-      <c r="F31" s="48" t="s">
+      <c r="F31" s="46" t="s">
         <v>122</v>
       </c>
-      <c r="G31" s="49" t="s">
+      <c r="G31" s="47" t="s">
         <v>123</v>
       </c>
       <c r="H31" t="s">
         <v>124</v>
       </c>
-      <c r="I31" s="69" t="s">
+      <c r="I31" t="s">
         <v>125</v>
       </c>
       <c r="J31" t="s">
@@ -6021,7 +5972,7 @@
         <f>消息模板!$E$12</f>
         <v>hmsg_message_template-12</v>
       </c>
-      <c r="G63" s="70" t="s">
+      <c r="G63" s="67" t="s">
         <v>231</v>
       </c>
       <c r="J63" t="s">
@@ -6075,7 +6026,7 @@
         <f>消息模板!$E$13</f>
         <v>hmsg_message_template-13</v>
       </c>
-      <c r="G66" s="70" t="s">
+      <c r="G66" s="67" t="s">
         <v>232</v>
       </c>
       <c r="J66" t="s">
@@ -6237,7 +6188,7 @@
         <f>消息模板!$E$14</f>
         <v>hmsg_message_template-14</v>
       </c>
-      <c r="G75" s="70" t="s">
+      <c r="G75" s="67" t="s">
         <v>232</v>
       </c>
       <c r="J75" t="s">
@@ -6255,7 +6206,7 @@
         <f>消息模板!$E$14</f>
         <v>hmsg_message_template-14</v>
       </c>
-      <c r="G76" s="70" t="s">
+      <c r="G76" s="67" t="s">
         <v>231</v>
       </c>
       <c r="J76" t="s">
@@ -7883,27 +7834,27 @@
   <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="35" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:11">
-      <c r="E4" s="38" t="s">
+      <c r="E4" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="F4" s="39" t="s">
+      <c r="F4" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="G4" s="40" t="s">
+      <c r="G4" s="38" t="s">
         <v>49</v>
       </c>
     </row>
@@ -7917,19 +7868,19 @@
       <c r="C7" t="s">
         <v>139</v>
       </c>
-      <c r="D7" s="50" t="s">
+      <c r="D7" s="48" t="s">
         <v>140</v>
       </c>
-      <c r="E7" s="51" t="s">
+      <c r="E7" s="49" t="s">
         <v>141</v>
       </c>
-      <c r="F7" s="52" t="s">
+      <c r="F7" s="50" t="s">
         <v>142</v>
       </c>
-      <c r="G7" s="53" t="s">
+      <c r="G7" s="51" t="s">
         <v>143</v>
       </c>
-      <c r="H7" s="54" t="s">
+      <c r="H7" s="52" t="s">
         <v>144</v>
       </c>
       <c r="I7" t="s">
@@ -8182,22 +8133,22 @@
       <c r="C19" t="s">
         <v>163</v>
       </c>
-      <c r="D19" s="55" t="s">
+      <c r="D19" s="53" t="s">
         <v>164</v>
       </c>
-      <c r="E19" s="56" t="s">
+      <c r="E19" s="54" t="s">
         <v>165</v>
       </c>
-      <c r="F19" s="57" t="s">
+      <c r="F19" s="55" t="s">
         <v>166</v>
       </c>
-      <c r="G19" s="58" t="s">
+      <c r="G19" s="56" t="s">
         <v>167</v>
       </c>
       <c r="H19" t="s">
         <v>168</v>
       </c>
-      <c r="I19" s="59" t="s">
+      <c r="I19" s="57" t="s">
         <v>169</v>
       </c>
       <c r="J19" t="s">
@@ -8241,22 +8192,22 @@
       <c r="C22" t="s">
         <v>176</v>
       </c>
-      <c r="D22" s="60" t="s">
+      <c r="D22" s="58" t="s">
         <v>164</v>
       </c>
-      <c r="E22" s="61" t="s">
+      <c r="E22" s="59" t="s">
         <v>165</v>
       </c>
-      <c r="F22" s="62" t="s">
+      <c r="F22" s="60" t="s">
         <v>166</v>
       </c>
-      <c r="G22" s="63" t="s">
+      <c r="G22" s="61" t="s">
         <v>167</v>
       </c>
       <c r="H22" t="s">
         <v>168</v>
       </c>
-      <c r="I22" s="64" t="s">
+      <c r="I22" s="62" t="s">
         <v>169</v>
       </c>
       <c r="J22" t="s">
@@ -8279,16 +8230,16 @@
       <c r="C24" t="s">
         <v>177</v>
       </c>
-      <c r="D24" s="65" t="s">
+      <c r="D24" s="63" t="s">
         <v>164</v>
       </c>
-      <c r="E24" s="66" t="s">
+      <c r="E24" s="64" t="s">
         <v>165</v>
       </c>
-      <c r="F24" s="67" t="s">
+      <c r="F24" s="65" t="s">
         <v>166</v>
       </c>
-      <c r="G24" s="68" t="s">
+      <c r="G24" s="66" t="s">
         <v>167</v>
       </c>
       <c r="H24" t="s">

</xml_diff>